<commit_message>
added an option for defoliation when PLC_TL is > 10 % : -added this parameter in modeling options - modified "update.LAIandStocks"
</commit_message>
<xml_diff>
--- a/documentation/soil-root-calibration.xlsx
+++ b/documentation/soil-root-calibration.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruffault/Dropbox/Mon Mac (MacBook-Pro-de-Julien.local)/Desktop/SurEau-Ecos_V4.0/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{D9361080-F3F5-5148-96E7-9B8EEDA37119}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE8D31E-28D9-B645-A57F-7DC59D1D57B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5180" yWindow="1800" windowWidth="28040" windowHeight="17440" activeTab="1" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
+    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -3036,8 +3036,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B673C9AC-1A9D-EA45-B245-5C46BCC162EE}">
   <dimension ref="B1:Y43"/>
   <sheetViews>
-    <sheetView topLeftCell="I1" zoomScale="162" zoomScaleNormal="218" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="124" zoomScaleNormal="218" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3095,7 +3095,7 @@
         <v>1</v>
       </c>
       <c r="C2" s="13">
-        <v>20</v>
+        <v>30</v>
       </c>
       <c r="D2" s="13" t="s">
         <v>6</v>
@@ -3402,14 +3402,14 @@
       </c>
       <c r="N15" s="2">
         <f>(C2*0.01)*(1-C5/100)</f>
-        <v>0.12</v>
+        <v>0.18</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>29</v>
       </c>
       <c r="Q15" s="2">
         <f>C2*0.01</f>
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="T15" s="2">
         <v>0.22</v>
@@ -3435,14 +3435,14 @@
       </c>
       <c r="N16" s="2">
         <f>0.01*(C3-C2)*(1-C6/100)</f>
-        <v>0.15999999999999998</v>
+        <v>0.13999999999999999</v>
       </c>
       <c r="P16" s="2" t="s">
         <v>30</v>
       </c>
       <c r="Q16" s="2">
         <f>(C3-C2)*0.01</f>
-        <v>0.8</v>
+        <v>0.70000000000000007</v>
       </c>
       <c r="T16" s="2">
         <v>0.23</v>
@@ -3505,7 +3505,7 @@
       </c>
       <c r="N18" s="2">
         <f>SUM(N15:N17)</f>
-        <v>0.57999999999999985</v>
+        <v>0.61999999999999988</v>
       </c>
       <c r="T18" s="2">
         <v>0.25</v>
@@ -3551,14 +3551,14 @@
     <row r="21" spans="2:21" x14ac:dyDescent="0.2">
       <c r="M21" s="2">
         <f>1/(SQRT(3.14*I32))</f>
-        <v>5.9236551862672099E-3</v>
+        <v>6.3314748259089542E-3</v>
       </c>
       <c r="N21" s="2" t="s">
         <v>36</v>
       </c>
       <c r="O21" s="2">
         <f>(2*3.14*F32)/LN(M21/C$12)</f>
-        <v>2018.5434593421749</v>
+        <v>2599.2515491885233</v>
       </c>
       <c r="R21" s="2" t="s">
         <v>39</v>
@@ -3587,18 +3587,18 @@
       </c>
       <c r="I22" s="2">
         <f>F32/Q15</f>
-        <v>5445.5539042270721</v>
+        <v>4766.6342959230669</v>
       </c>
       <c r="M22" s="2">
         <f>1/(SQRT(3.14*I33))</f>
-        <v>6.5583227411875273E-3</v>
+        <v>7.2690340564040236E-3</v>
       </c>
       <c r="N22" s="2" t="s">
         <v>37</v>
       </c>
       <c r="O22" s="2">
         <f>(2*3.14*F33)/LN(M22/C$12)</f>
-        <v>2131.6577553675038</v>
+        <v>1474.8233134415109</v>
       </c>
       <c r="R22" s="2" t="s">
         <v>41</v>
@@ -3617,7 +3617,7 @@
       </c>
       <c r="I23" s="2">
         <f>F33/Q16</f>
-        <v>1480.8626439273041</v>
+        <v>1205.4437245861966</v>
       </c>
       <c r="M23" s="2">
         <f>1/(SQRT(3.14*I34))</f>
@@ -3743,28 +3743,28 @@
       </c>
       <c r="C32" s="2">
         <f>1-C$8^C2</f>
-        <v>0.45620565707325289</v>
+        <v>0.5989929314568424</v>
       </c>
       <c r="E32" s="2" t="s">
         <v>16</v>
       </c>
       <c r="F32" s="2">
         <f>C$24*C32</f>
-        <v>1089.1107808454144</v>
+        <v>1429.9902887769199</v>
       </c>
       <c r="H32" s="2" t="s">
         <v>15</v>
       </c>
       <c r="I32" s="2">
         <f>F32/N15</f>
-        <v>9075.923173711788</v>
+        <v>7944.3904932051109</v>
       </c>
       <c r="K32" s="2" t="s">
         <v>23</v>
       </c>
       <c r="L32" s="2">
         <f>C$13*(F32)/F$35</f>
-        <v>0.79836398208161208</v>
+        <v>1.0482429899369616</v>
       </c>
       <c r="T32" s="2">
         <v>0.39</v>
@@ -3780,28 +3780,28 @@
       </c>
       <c r="C33" s="2">
         <f>(1-C$8^C3)-C32</f>
-        <v>0.49624183500134145</v>
+        <v>0.35345456061775193</v>
       </c>
       <c r="E33" s="2" t="s">
         <v>17</v>
       </c>
       <c r="F33" s="2">
         <f>C$24*C33</f>
-        <v>1184.6901151418433</v>
+        <v>843.81060721033771</v>
       </c>
       <c r="H33" s="2" t="s">
         <v>21</v>
       </c>
       <c r="I33" s="2">
         <f>F33/N16</f>
-        <v>7404.3132196365214</v>
+        <v>6027.2186229309846</v>
       </c>
       <c r="K33" s="2" t="s">
         <v>24</v>
       </c>
       <c r="L33" s="2">
         <f>C$13*(F33)/F$35</f>
-        <v>0.86842765170608671</v>
+        <v>0.61854864385073705</v>
       </c>
       <c r="T33" s="2">
         <v>0.4</v>
@@ -3992,7 +3992,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3ABBAEF3-718F-D345-A528-FF8E58100BB4}">
   <dimension ref="B2:K43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+    <sheetView zoomScale="135" workbookViewId="0">
       <selection activeCell="G7" sqref="G7"/>
     </sheetView>
   </sheetViews>
@@ -4046,19 +4046,19 @@
       </c>
       <c r="E3" s="2">
         <f>D3*Feuil1!I$22*Feuil1!C$17</f>
-        <v>1.5307236281378128E-2</v>
+        <v>1.3398820160053337E-2</v>
       </c>
       <c r="F3" s="2">
         <f>E3*1000</f>
-        <v>15.307236281378128</v>
+        <v>13.398820160053337</v>
       </c>
       <c r="G3" s="2">
         <f>1/((1/E3)+(1/Feuil1!L$32))</f>
-        <v>1.5019268024315593E-2</v>
+        <v>1.322971568434976E-2</v>
       </c>
       <c r="H3" s="2">
         <f>1/((1/F3)+(1/Feuil1!L$32))</f>
-        <v>0.75878861466539094</v>
+        <v>0.97218508428900852</v>
       </c>
       <c r="I3" s="2"/>
       <c r="J3" s="2"/>
@@ -4078,19 +4078,19 @@
       </c>
       <c r="E4" s="2">
         <f>D4*Feuil1!I$22*Feuil1!C$17</f>
-        <v>1.5307236281378128E-2</v>
+        <v>1.3398820160053337E-2</v>
       </c>
       <c r="F4" s="2">
         <f t="shared" ref="F4:F21" si="0">E4*1000</f>
-        <v>15.307236281378128</v>
+        <v>13.398820160053337</v>
       </c>
       <c r="G4" s="2">
         <f>1/((1/E4)+(1/Feuil1!L$32))</f>
-        <v>1.5019268024315593E-2</v>
+        <v>1.322971568434976E-2</v>
       </c>
       <c r="H4" s="2">
         <f>1/((1/F4)+(1/Feuil1!L$32))</f>
-        <v>0.75878861466539094</v>
+        <v>0.97218508428900852</v>
       </c>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
@@ -4110,19 +4110,19 @@
       </c>
       <c r="E5" s="2">
         <f>D5*Feuil1!I$22*Feuil1!C$17</f>
-        <v>0.3479798600514627</v>
+        <v>0.30459577930617171</v>
       </c>
       <c r="F5" s="2">
         <f t="shared" si="0"/>
-        <v>347.97986005146271</v>
+        <v>304.59577930617172</v>
       </c>
       <c r="G5" s="2">
         <f>1/((1/E5)+(1/Feuil1!L$32))</f>
-        <v>0.24234839194315433</v>
+        <v>0.2360151096207217</v>
       </c>
       <c r="H5" s="2">
         <f>1/((1/F5)+(1/Feuil1!L$32))</f>
-        <v>0.79653650260048514</v>
+        <v>1.0446479143398755</v>
       </c>
       <c r="I5" s="2"/>
       <c r="J5" s="2"/>
@@ -4142,19 +4142,19 @@
       </c>
       <c r="E6" s="2">
         <f>D6*Feuil1!I$22*Feuil1!C$17</f>
-        <v>2.174538669597879</v>
+        <v>1.9034299875849603</v>
       </c>
       <c r="F6" s="2">
         <f t="shared" si="0"/>
-        <v>2174.5386695978791</v>
+        <v>1903.4299875849604</v>
       </c>
       <c r="G6" s="2">
         <f>1/((1/E6)+(1/Feuil1!L$32))</f>
-        <v>0.58396575833717534</v>
+        <v>0.6759750001156466</v>
       </c>
       <c r="H6" s="2">
         <f>1/((1/F6)+(1/Feuil1!L$32))</f>
-        <v>0.79807097688837259</v>
+        <v>1.0476660269933524</v>
       </c>
       <c r="I6" s="2"/>
       <c r="J6" s="2"/>
@@ -4174,19 +4174,19 @@
       </c>
       <c r="E7" s="2">
         <f>D7*Feuil1!I$22*Feuil1!C$17</f>
-        <v>8.0245981629295375</v>
+        <v>7.0241384966788463</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="0"/>
-        <v>8024.5981629295375</v>
+        <v>7024.1384966788464</v>
       </c>
       <c r="G7" s="2">
         <f>1/((1/E7)+(1/Feuil1!L$32))</f>
-        <v>0.72612236555766374</v>
+        <v>0.91212289108213929</v>
       </c>
       <c r="H7" s="2">
         <f>1/((1/F7)+(1/Feuil1!L$32))</f>
-        <v>0.79828456107783397</v>
+        <v>1.0480865793806773</v>
       </c>
       <c r="I7" s="2"/>
       <c r="J7" s="2"/>
@@ -4206,19 +4206,19 @@
       </c>
       <c r="E8" s="2">
         <f>D8*Feuil1!I$22*Feuil1!C$17</f>
-        <v>22.225560429972838</v>
+        <v>19.454608374987</v>
       </c>
       <c r="F8" s="2">
         <f t="shared" si="0"/>
-        <v>22225.560429972837</v>
+        <v>19454.608374987001</v>
       </c>
       <c r="G8" s="2">
         <f>1/((1/E8)+(1/Feuil1!L$32))</f>
-        <v>0.77068038494682056</v>
+        <v>0.99464979226925476</v>
       </c>
       <c r="H8" s="2">
         <f>1/((1/F8)+(1/Feuil1!L$32))</f>
-        <v>0.79833530509255635</v>
+        <v>1.0481865121018759</v>
       </c>
       <c r="I8" s="2"/>
       <c r="K8" s="2"/>
@@ -4237,19 +4237,19 @@
       </c>
       <c r="E9" s="2">
         <f>D9*Feuil1!I$22*Feuil1!C$17</f>
-        <v>51.416935365328584</v>
+        <v>45.006574503539269</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="0"/>
-        <v>51416.935365328587</v>
+        <v>45006.574503539268</v>
       </c>
       <c r="G9" s="2">
         <f>1/((1/E9)+(1/Feuil1!L$32))</f>
-        <v>0.78615711827251245</v>
+        <v>1.0243841750343159</v>
       </c>
       <c r="H9" s="2">
         <f>1/((1/F9)+(1/Feuil1!L$32))</f>
-        <v>0.79835158587116772</v>
+        <v>1.0482185759977465</v>
       </c>
       <c r="I9" s="2"/>
       <c r="J9" s="2"/>
@@ -4269,19 +4269,19 @@
       </c>
       <c r="E10" s="2">
         <f>D10*Feuil1!I$22*Feuil1!C$17</f>
-        <v>105.20673442807836</v>
+        <v>92.090178025356906</v>
       </c>
       <c r="F10" s="2">
         <f t="shared" si="0"/>
-        <v>105206.73442807836</v>
+        <v>92090.178025356901</v>
       </c>
       <c r="G10" s="2">
         <f>1/((1/E10)+(1/Feuil1!L$32))</f>
-        <v>0.79235120479594801</v>
+        <v>1.0364453520344299</v>
       </c>
       <c r="H10" s="2">
         <f>1/((1/F10)+(1/Feuil1!L$32))</f>
-        <v>0.79835792372218695</v>
+        <v>1.0482310581448628</v>
       </c>
       <c r="I10" s="2"/>
       <c r="J10" s="2"/>
@@ -4301,19 +4301,19 @@
       </c>
       <c r="E11" s="2">
         <f>D11*Feuil1!I$22*Feuil1!C$17</f>
-        <v>197.06194118412236</v>
+        <v>172.49341826187225</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="0"/>
-        <v>197061.94118412235</v>
+        <v>172493.41826187226</v>
       </c>
       <c r="G11" s="2">
         <f>1/((1/E11)+(1/Feuil1!L$32))</f>
-        <v>0.79514259289316525</v>
+        <v>1.0419112920724494</v>
       </c>
       <c r="H11" s="2">
         <f>1/((1/F11)+(1/Feuil1!L$32))</f>
-        <v>0.79836074765459997</v>
+        <v>1.0482366198000626</v>
       </c>
       <c r="I11" s="2"/>
       <c r="J11" s="2"/>
@@ -4333,19 +4333,19 @@
       </c>
       <c r="E12" s="2">
         <f>D12*Feuil1!I$22*Feuil1!C$17</f>
-        <v>345.57473327086115</v>
+        <v>302.49050957602378</v>
       </c>
       <c r="F12" s="2">
         <f t="shared" si="0"/>
-        <v>345574.73327086115</v>
+        <v>302490.50957602379</v>
       </c>
       <c r="G12" s="2">
         <f>1/((1/E12)+(1/Feuil1!L$32))</f>
-        <v>0.79652381304729547</v>
+        <v>1.0446229797845077</v>
       </c>
       <c r="H12" s="2">
         <f>1/((1/F12)+(1/Feuil1!L$32))</f>
-        <v>0.79836213766558861</v>
+        <v>1.0482393573947053</v>
       </c>
       <c r="I12" s="2"/>
       <c r="J12" s="2"/>
@@ -4365,19 +4365,19 @@
       </c>
       <c r="E13" s="2">
         <f>D13*Feuil1!I$22*Feuil1!C$17</f>
-        <v>576.34390828338508</v>
+        <v>504.48874215300884</v>
       </c>
       <c r="F13" s="2">
         <f t="shared" si="0"/>
-        <v>576343.9082833851</v>
+        <v>504488.74215300882</v>
       </c>
       <c r="G13" s="2">
         <f>1/((1/E13)+(1/Feuil1!L$32))</f>
-        <v>0.79725960092896619</v>
+        <v>1.0460694331087874</v>
       </c>
       <c r="H13" s="2">
         <f>1/((1/F13)+(1/Feuil1!L$32))</f>
-        <v>0.79836287617217883</v>
+        <v>1.0482408118683726</v>
       </c>
       <c r="I13" s="2"/>
       <c r="J13" s="2"/>
@@ -4397,19 +4397,19 @@
       </c>
       <c r="E14" s="2">
         <f>D14*Feuil1!I$22*Feuil1!C$17</f>
-        <v>924.90583296470948</v>
+        <v>809.59401769701753</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="0"/>
-        <v>924905.83296470949</v>
+        <v>809594.01769701752</v>
       </c>
       <c r="G14" s="2">
         <f>1/((1/E14)+(1/Feuil1!L$32))</f>
-        <v>0.79767544134690715</v>
+        <v>1.0468875050094661</v>
       </c>
       <c r="H14" s="2">
         <f>1/((1/F14)+(1/Feuil1!L$32))</f>
-        <v>0.79836329294713493</v>
+        <v>1.0482416326987418</v>
       </c>
       <c r="I14" s="2"/>
       <c r="J14" s="2"/>
@@ -4429,19 +4429,19 @@
       </c>
       <c r="E15" s="2">
         <f>D15*Feuil1!I$22*Feuil1!C$17</f>
-        <v>1441.562104286993</v>
+        <v>1261.8366261444094</v>
       </c>
       <c r="F15" s="2">
         <f t="shared" si="0"/>
-        <v>1441562.1042869929</v>
+        <v>1261836.6261444094</v>
       </c>
       <c r="G15" s="2">
         <f>1/((1/E15)+(1/Feuil1!L$32))</f>
-        <v>0.7979220779516063</v>
+        <v>1.0473729079581464</v>
       </c>
       <c r="H15" s="2">
         <f>1/((1/F15)+(1/Feuil1!L$32))</f>
-        <v>0.79836353993299214</v>
+        <v>1.0482421191329048</v>
       </c>
       <c r="I15" s="2"/>
       <c r="J15" s="2"/>
@@ -4461,19 +4461,19 @@
       </c>
       <c r="E16" s="2">
         <f>D16*Feuil1!I$22*Feuil1!C$17</f>
-        <v>2199.906173092972</v>
+        <v>1925.6348200571533</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="0"/>
-        <v>2199906.173092972</v>
+        <v>1925634.8200571532</v>
       </c>
       <c r="G16" s="2">
         <f>1/((1/E16)+(1/Feuil1!L$32))</f>
-        <v>0.7980743543568779</v>
+        <v>1.0476726764344315</v>
       </c>
       <c r="H16" s="2">
         <f>1/((1/F16)+(1/Feuil1!L$32))</f>
-        <v>0.79836369234888427</v>
+        <v>1.0482424193133126</v>
       </c>
       <c r="I16" s="2"/>
       <c r="J16" s="2"/>
@@ -4493,19 +4493,19 @@
       </c>
       <c r="E17" s="2">
         <f>D17*Feuil1!I$22*Feuil1!C$17</f>
-        <v>3313.3356538928456</v>
+        <v>2900.2484668255247</v>
       </c>
       <c r="F17" s="2">
         <f t="shared" si="0"/>
-        <v>3313335.6538928454</v>
+        <v>2900248.4668255248</v>
       </c>
       <c r="G17" s="2">
         <f>1/((1/E17)+(1/Feuil1!L$32))</f>
-        <v>0.79817165882478325</v>
+        <v>1.04786425812293</v>
       </c>
       <c r="H17" s="2">
         <f>1/((1/F17)+(1/Feuil1!L$32))</f>
-        <v>0.79836378971206046</v>
+        <v>1.0482426110683987</v>
       </c>
       <c r="I17" s="2"/>
       <c r="J17" s="2"/>
@@ -4525,19 +4525,19 @@
       </c>
       <c r="E18" s="2">
         <f>D18*Feuil1!I$22*Feuil1!C$17</f>
-        <v>4971.4348037962272</v>
+        <v>4351.6255742737249</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="0"/>
-        <v>4971434.8037962271</v>
+        <v>4351625.574273725</v>
       </c>
       <c r="G18" s="2">
         <f>1/((1/E18)+(1/Feuil1!L$32))</f>
-        <v>0.79823579319215787</v>
+        <v>1.0479905443340787</v>
       </c>
       <c r="H18" s="2">
         <f>1/((1/F18)+(1/Feuil1!L$32))</f>
-        <v>0.79836385387215736</v>
+        <v>1.0482427374306091</v>
       </c>
       <c r="I18" s="2"/>
       <c r="J18" s="2"/>
@@ -4557,19 +4557,19 @@
       </c>
       <c r="E19" s="2">
         <f>D19*Feuil1!I$22*Feuil1!C$17</f>
-        <v>7537.6763297594134</v>
+        <v>6597.9232116514049</v>
       </c>
       <c r="F19" s="2">
         <f t="shared" si="0"/>
-        <v>7537676.3297594134</v>
+        <v>6597923.2116514053</v>
       </c>
       <c r="G19" s="2">
         <f>1/((1/E19)+(1/Feuil1!L$32))</f>
-        <v>0.79827943115138023</v>
+        <v>1.0480764771139399</v>
       </c>
       <c r="H19" s="2">
         <f>1/((1/F19)+(1/Feuil1!L$32))</f>
-        <v>0.79836389752173542</v>
+        <v>1.0482428233977104</v>
       </c>
       <c r="I19" s="2"/>
       <c r="J19" s="2"/>
@@ -4589,19 +4589,19 @@
       </c>
       <c r="E20" s="2">
         <f>D20*Feuil1!I$22*Feuil1!C$17</f>
-        <v>11925.345276016353</v>
+        <v>10438.563419463926</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="0"/>
-        <v>11925345.276016353</v>
+        <v>10438563.419463927</v>
       </c>
       <c r="G20" s="2">
         <f>1/((1/E20)+(1/Feuil1!L$32))</f>
-        <v>0.79831053772716487</v>
+        <v>1.0481377356994017</v>
       </c>
       <c r="H20" s="2">
         <f>1/((1/F20)+(1/Feuil1!L$32))</f>
-        <v>0.79836392863368322</v>
+        <v>1.048242884672165</v>
       </c>
       <c r="I20" s="2"/>
       <c r="J20" s="2"/>
@@ -4620,19 +4620,19 @@
       </c>
       <c r="E21" s="2">
         <f>D21*Feuil1!I$22*Feuil1!C$17</f>
-        <v>18958.483541270925</v>
+        <v>16594.851402787026</v>
       </c>
       <c r="F21" s="2">
         <f t="shared" si="0"/>
-        <v>18958483.541270927</v>
+        <v>16594851.402787026</v>
       </c>
       <c r="G21" s="2">
         <f>1/((1/E21)+(1/Feuil1!L$32))</f>
-        <v>0.7983303634534874</v>
+        <v>1.0481767800062314</v>
       </c>
       <c r="H21" s="2">
         <f>1/((1/F21)+(1/Feuil1!L$32))</f>
-        <v>0.79836394846156966</v>
+        <v>1.0482429237228528</v>
       </c>
       <c r="I21" s="2"/>
       <c r="J21" s="2"/>

</xml_diff>

<commit_message>
updated initialisation + added script for sensitivity analyses
</commit_message>
<xml_diff>
--- a/documentation/soil-root-calibration.xlsx
+++ b/documentation/soil-root-calibration.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruffault/Dropbox/Mon Mac (MacBook-Pro-de-Julien.local)/Desktop/SurEau-Ecos_V4.0/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AE8D31E-28D9-B645-A57F-7DC59D1D57B2}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFAE4D8-B822-2845-AEA7-DD74E9406ADB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="760" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
+    <workbookView xWindow="60" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
     <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="107">
   <si>
     <t>Depth_layer_3</t>
   </si>
@@ -433,6 +433,9 @@
   </si>
   <si>
     <t>cm3.cm-3</t>
+  </si>
+  <si>
+    <t>Van Genuchten</t>
   </si>
 </sst>
 </file>
@@ -496,7 +499,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="9">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -590,11 +593,48 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -647,6 +687,15 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" textRotation="90"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -674,8 +723,8 @@
       <xdr:rowOff>24679</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2069469" cy="173477"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="ZoneTexte 1">
@@ -808,7 +857,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="2" name="ZoneTexte 1">
@@ -875,8 +924,8 @@
       <xdr:rowOff>16076</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2069469" cy="173477"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="ZoneTexte 2">
@@ -965,7 +1014,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="3" name="ZoneTexte 2">
@@ -1040,8 +1089,8 @@
       <xdr:rowOff>119038</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2069469" cy="339963"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="ZoneTexte 4">
@@ -1294,7 +1343,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="5" name="ZoneTexte 4">
@@ -1388,8 +1437,8 @@
       <xdr:rowOff>61999</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="863106" cy="463550"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="ZoneTexte 6">
@@ -1431,6 +1480,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -1536,7 +1586,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="7" name="ZoneTexte 6">
@@ -1607,8 +1657,8 @@
       <xdr:rowOff>146493</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2807509" cy="463550"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="ZoneTexte 7">
@@ -1933,7 +1983,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="8" name="ZoneTexte 7">
@@ -2016,9 +2066,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>913528</xdr:colOff>
-      <xdr:row>15</xdr:row>
-      <xdr:rowOff>277163</xdr:rowOff>
+      <xdr:colOff>881578</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>205275</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2069469" cy="539198"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2036,7 +2086,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10204183" y="4223234"/>
+              <a:off x="12255666" y="3687791"/>
               <a:ext cx="2069469" cy="539198"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2064,6 +2114,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2296,7 +2347,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10204183" y="4223234"/>
+              <a:off x="12255666" y="3687791"/>
               <a:ext cx="2069469" cy="539198"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2324,6 +2375,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="fr-FR" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -2341,9 +2393,9 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>6</xdr:col>
-      <xdr:colOff>922261</xdr:colOff>
-      <xdr:row>14</xdr:row>
-      <xdr:rowOff>153938</xdr:rowOff>
+      <xdr:colOff>906286</xdr:colOff>
+      <xdr:row>12</xdr:row>
+      <xdr:rowOff>385574</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2941342" cy="764199"/>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -2361,7 +2413,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10212916" y="3669117"/>
+              <a:off x="12280374" y="2989473"/>
               <a:ext cx="2941342" cy="764199"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2389,6 +2441,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a14:m>
                 <m:oMathPara xmlns:m="http://schemas.openxmlformats.org/officeDocument/2006/math">
                   <m:oMathParaPr>
@@ -2692,7 +2745,7 @@
           </xdr:nvSpPr>
           <xdr:spPr>
             <a:xfrm>
-              <a:off x="10212916" y="3669117"/>
+              <a:off x="12280374" y="2989473"/>
               <a:ext cx="2941342" cy="764199"/>
             </a:xfrm>
             <a:prstGeom prst="rect">
@@ -2720,6 +2773,7 @@
             </a:bodyPr>
             <a:lstStyle/>
             <a:p>
+              <a:pPr/>
               <a:r>
                 <a:rPr lang="fr-FR" sz="1100" b="0" i="0">
                   <a:latin typeface="Cambria Math" panose="02040503050406030204" pitchFamily="18" charset="0"/>
@@ -3034,17 +3088,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B673C9AC-1A9D-EA45-B245-5C46BCC162EE}">
-  <dimension ref="B1:Y43"/>
+  <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" zoomScale="124" zoomScaleNormal="218" workbookViewId="0">
-      <selection activeCell="E27" sqref="E27"/>
+    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="218" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20:C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="10.83203125" style="2"/>
-    <col min="2" max="2" width="20.83203125" style="2" customWidth="1"/>
-    <col min="3" max="3" width="13.6640625" style="2" customWidth="1"/>
+    <col min="2" max="2" width="37.6640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="24.33203125" style="2" customWidth="1"/>
     <col min="4" max="4" width="23.1640625" style="2" customWidth="1"/>
     <col min="5" max="5" width="42.6640625" style="2" customWidth="1"/>
     <col min="6" max="6" width="10.6640625" style="2" customWidth="1"/>
@@ -3067,7 +3121,7 @@
     <col min="26" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:25" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:25" ht="18" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B1" s="3" t="s">
         <v>58</v>
       </c>
@@ -3090,7 +3144,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="2" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B2" s="12" t="s">
         <v>1</v>
       </c>
@@ -3128,7 +3182,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B3" s="12" t="s">
         <v>2</v>
       </c>
@@ -3155,7 +3209,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B4" s="12" t="s">
         <v>0</v>
       </c>
@@ -3172,11 +3226,11 @@
         <v>0.11</v>
       </c>
       <c r="U4" s="2">
-        <f t="shared" ref="U4:U48" si="0">(T4-C$19)/(C$18-C$19)</f>
+        <f t="shared" ref="U4:U43" si="0">(T4-C$19)/(C$18-C$19)</f>
         <v>5.5555555555555525E-2</v>
       </c>
     </row>
-    <row r="5" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B5" s="12" t="s">
         <v>94</v>
       </c>
@@ -3197,7 +3251,7 @@
         <v>0.11111111111111105</v>
       </c>
     </row>
-    <row r="6" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B6" s="12" t="s">
         <v>95</v>
       </c>
@@ -3218,7 +3272,7 @@
         <v>0.16666666666666663</v>
       </c>
     </row>
-    <row r="7" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B7" s="12" t="s">
         <v>96</v>
       </c>
@@ -3239,7 +3293,7 @@
         <v>0.22222222222222224</v>
       </c>
     </row>
-    <row r="8" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B8" s="12" t="s">
         <v>86</v>
       </c>
@@ -3260,7 +3314,7 @@
         <v>0.27777777777777768</v>
       </c>
     </row>
-    <row r="9" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="s">
         <v>3</v>
       </c>
@@ -3281,7 +3335,7 @@
         <v>0.33333333333333326</v>
       </c>
     </row>
-    <row r="10" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B10" s="12" t="s">
         <v>97</v>
       </c>
@@ -3302,7 +3356,7 @@
         <v>0.3888888888888889</v>
       </c>
     </row>
-    <row r="11" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B11" s="12" t="s">
         <v>8</v>
       </c>
@@ -3323,7 +3377,7 @@
         <v>0.44444444444444431</v>
       </c>
     </row>
-    <row r="12" spans="2:25" ht="17" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:25" ht="17" x14ac:dyDescent="0.2">
       <c r="B12" s="12" t="s">
         <v>93</v>
       </c>
@@ -3344,7 +3398,7 @@
         <v>0.49999999999999994</v>
       </c>
     </row>
-    <row r="13" spans="2:25" ht="35" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:25" ht="35" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B13" s="15" t="s">
         <v>92</v>
       </c>
@@ -3365,7 +3419,10 @@
         <v>0.55555555555555547</v>
       </c>
     </row>
-    <row r="14" spans="2:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>106</v>
+      </c>
       <c r="B14" s="6" t="s">
         <v>51</v>
       </c>
@@ -3386,7 +3443,8 @@
         <v>0.61111111111111094</v>
       </c>
     </row>
-    <row r="15" spans="2:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="A15" s="19"/>
       <c r="B15" s="6" t="s">
         <v>54</v>
       </c>
@@ -3419,7 +3477,8 @@
         <v>0.66666666666666652</v>
       </c>
     </row>
-    <row r="16" spans="2:25" ht="34" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:25" ht="34" x14ac:dyDescent="0.2">
+      <c r="A16" s="19"/>
       <c r="B16" s="6" t="s">
         <v>52</v>
       </c>
@@ -3452,7 +3511,8 @@
         <v>0.72222222222222221</v>
       </c>
     </row>
-    <row r="17" spans="2:21" ht="34" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:21" ht="34" x14ac:dyDescent="0.2">
+      <c r="A17" s="19"/>
       <c r="B17" s="6" t="s">
         <v>53</v>
       </c>
@@ -3487,7 +3547,8 @@
         <v>0.77777777777777757</v>
       </c>
     </row>
-    <row r="18" spans="2:21" ht="17" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:21" ht="17" x14ac:dyDescent="0.2">
+      <c r="A18" s="19"/>
       <c r="B18" s="6" t="s">
         <v>55</v>
       </c>
@@ -3515,7 +3576,8 @@
         <v>0.83333333333333326</v>
       </c>
     </row>
-    <row r="19" spans="2:21" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:21" ht="18" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A19" s="20"/>
       <c r="B19" s="7" t="s">
         <v>56</v>
       </c>
@@ -3536,7 +3598,7 @@
         <v>0.88888888888888884</v>
       </c>
     </row>
-    <row r="20" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:21" x14ac:dyDescent="0.2">
       <c r="M20" s="2" t="s">
         <v>20</v>
       </c>
@@ -3548,7 +3610,7 @@
         <v>0.94444444444444442</v>
       </c>
     </row>
-    <row r="21" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:21" x14ac:dyDescent="0.2">
       <c r="M21" s="2">
         <f>1/(SQRT(3.14*I32))</f>
         <v>6.3314748259089542E-3</v>
@@ -3571,7 +3633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B22" s="2" t="s">
         <v>9</v>
       </c>
@@ -3611,7 +3673,7 @@
         <v>1.0555555555555554</v>
       </c>
     </row>
-    <row r="23" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:21" x14ac:dyDescent="0.2">
       <c r="H23" s="2" t="s">
         <v>34</v>
       </c>
@@ -3641,7 +3703,7 @@
         <v>1.1111111111111109</v>
       </c>
     </row>
-    <row r="24" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B24" s="2" t="s">
         <v>46</v>
       </c>
@@ -3667,7 +3729,7 @@
         <v>1.1666666666666665</v>
       </c>
     </row>
-    <row r="25" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:21" x14ac:dyDescent="0.2">
       <c r="T25" s="2">
         <v>0.32</v>
       </c>
@@ -3676,7 +3738,7 @@
         <v>1.2222222222222221</v>
       </c>
     </row>
-    <row r="26" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:21" x14ac:dyDescent="0.2">
       <c r="T26" s="2">
         <v>0.33</v>
       </c>
@@ -3685,7 +3747,7 @@
         <v>1.2777777777777777</v>
       </c>
     </row>
-    <row r="27" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B27" s="2" t="s">
         <v>98</v>
       </c>
@@ -3701,7 +3763,7 @@
         <v>1.3333333333333333</v>
       </c>
     </row>
-    <row r="28" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:21" x14ac:dyDescent="0.2">
       <c r="T28" s="2">
         <v>0.35</v>
       </c>
@@ -3710,7 +3772,7 @@
         <v>1.3888888888888886</v>
       </c>
     </row>
-    <row r="29" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:21" x14ac:dyDescent="0.2">
       <c r="T29" s="2">
         <v>0.36</v>
       </c>
@@ -3719,7 +3781,7 @@
         <v>1.4444444444444444</v>
       </c>
     </row>
-    <row r="30" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:21" x14ac:dyDescent="0.2">
       <c r="T30" s="2">
         <v>0.37</v>
       </c>
@@ -3728,7 +3790,7 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="31" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:21" x14ac:dyDescent="0.2">
       <c r="T31" s="2">
         <v>0.38</v>
       </c>
@@ -3737,7 +3799,7 @@
         <v>1.5555555555555556</v>
       </c>
     </row>
-    <row r="32" spans="2:21" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:21" x14ac:dyDescent="0.2">
       <c r="B32" s="2" t="s">
         <v>11</v>
       </c>
@@ -3983,6 +4045,9 @@
       </c>
     </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A14:A19"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
@@ -3993,7 +4058,7 @@
   <dimension ref="B2:K43"/>
   <sheetViews>
     <sheetView zoomScale="135" workbookViewId="0">
-      <selection activeCell="G7" sqref="G7"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
modified parameters name and update documentation
</commit_message>
<xml_diff>
--- a/documentation/soil-root-calibration.xlsx
+++ b/documentation/soil-root-calibration.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10411"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10509"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jruffault/Dropbox/Mon Mac (MacBook-Pro-de-Julien.local)/Desktop/SurEau-Ecos_V4.0/documentation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FFAE4D8-B822-2845-AEA7-DD74E9406ADB}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DEB6AA5F-CA7C-E64A-AE51-7D8B9444C80E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="60" yWindow="500" windowWidth="28040" windowHeight="17440" xr2:uid="{D9106142-DCBD-4E45-A888-1E539F445614}"/>
   </bookViews>
@@ -2071,8 +2071,8 @@
       <xdr:rowOff>205275</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2069469" cy="539198"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="ZoneTexte 8">
@@ -2333,7 +2333,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="9" name="ZoneTexte 8">
@@ -2398,8 +2398,8 @@
       <xdr:rowOff>385574</xdr:rowOff>
     </xdr:from>
     <xdr:ext cx="2941342" cy="764199"/>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" Requires="a14">
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main">
+      <mc:Choice Requires="a14">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="ZoneTexte 10">
@@ -2731,7 +2731,7 @@
           </xdr:txBody>
         </xdr:sp>
       </mc:Choice>
-      <mc:Fallback>
+      <mc:Fallback xmlns="">
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
             <xdr:cNvPr id="11" name="ZoneTexte 10">
@@ -3090,8 +3090,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B673C9AC-1A9D-EA45-B245-5C46BCC162EE}">
   <dimension ref="A1:Y43"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="114" zoomScaleNormal="218" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20:C21"/>
+    <sheetView tabSelected="1" zoomScale="125" zoomScaleNormal="218" workbookViewId="0">
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>